<commit_message>
Updates since I moved
</commit_message>
<xml_diff>
--- a/mpgcalc.xlsx
+++ b/mpgcalc.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiozygmunt/projects/mpg-calcuator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286E4F8C-7A1D-FF40-8CFE-B1AED2CD6234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AEFC63-B920-D041-9B70-7BC16E51760D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{E96B15E8-25ED-594B-AF36-006F4E18FFC7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" activeTab="1" xr2:uid="{E96B15E8-25ED-594B-AF36-006F4E18FFC7}"/>
   </bookViews>
   <sheets>
-    <sheet name="16 Escape (2)" sheetId="5" r:id="rId1"/>
-    <sheet name="16 Escape" sheetId="4" r:id="rId2"/>
-    <sheet name="cx5" sheetId="2" r:id="rId3"/>
-    <sheet name="cx3" sheetId="3" r:id="rId4"/>
+    <sheet name="FRC Robotics Short" sheetId="7" r:id="rId1"/>
+    <sheet name="FRC Robotics Long" sheetId="6" r:id="rId2"/>
+    <sheet name="2020 Escape Hybrid" sheetId="5" r:id="rId3"/>
+    <sheet name="16 Escape" sheetId="4" r:id="rId4"/>
+    <sheet name="cx5" sheetId="2" r:id="rId5"/>
+    <sheet name="cx3" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="53">
   <si>
     <t>MPG Calcuator</t>
   </si>
@@ -150,6 +152,51 @@
   </si>
   <si>
     <t>Ford Escape 2020 Hybrid</t>
+  </si>
+  <si>
+    <t>To or from FRC Event</t>
+  </si>
+  <si>
+    <t>To or from NEDO</t>
+  </si>
+  <si>
+    <t>combMPGNEDO</t>
+  </si>
+  <si>
+    <t>to or from NEDO</t>
+  </si>
+  <si>
+    <t>round trip NEDO</t>
+  </si>
+  <si>
+    <t>CostPerMileNEDO</t>
+  </si>
+  <si>
+    <t>CostPerTripNEDO</t>
+  </si>
+  <si>
+    <t>CostPerRoundTrNEDO</t>
+  </si>
+  <si>
+    <t>combMPGRCC</t>
+  </si>
+  <si>
+    <t>to or from RCC</t>
+  </si>
+  <si>
+    <t>round trip RCC</t>
+  </si>
+  <si>
+    <t>CostPerMileRCC</t>
+  </si>
+  <si>
+    <t>CostPerDirRCC</t>
+  </si>
+  <si>
+    <t>CostPerRoundTrRCC</t>
+  </si>
+  <si>
+    <t>To or from FRC Event from NEDO</t>
   </si>
 </sst>
 </file>
@@ -641,11 +688,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C462358-9A63-4D48-8958-D591B0DFAB04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56922D58-C711-594B-8303-26E18AA947FD}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="94" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,7 +712,7 @@
         <v>35</v>
       </c>
       <c r="F1" s="1">
-        <v>2.4700000000000002</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -678,11 +725,11 @@
         <v>19</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C4" s="14"/>
       <c r="E4" s="13" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="F4" s="14"/>
     </row>
@@ -692,13 +739,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -707,13 +754,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>9.1</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="5">
-        <v>4.5999999999999996</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -723,14 +770,14 @@
       </c>
       <c r="C7" s="7">
         <f>SUM(C5:C6)</f>
-        <v>9.1</v>
+        <v>330</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="7">
         <f>SUM(F5:F6)</f>
-        <v>4.5999999999999996</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -788,41 +835,41 @@
         <v>9</v>
       </c>
       <c r="F12" s="5">
-        <v>16.5</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5">
         <f>((C10*(C5/C7))+(C11*(C6/C7)))</f>
-        <v>37</v>
+        <v>42.81818181818182</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5">
         <f>((F10*(C5/C7))+(F11*(C6/C7)))</f>
-        <v>19</v>
+        <v>23.848484848484848</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C14" s="8">
         <f>((C10*(F5/F7))+(C11*(F6/F7)))</f>
-        <v>37</v>
+        <v>41.838709677419352</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F14" s="7">
         <f>((F10*(F5/F7))+(F11*(F6/F7)))</f>
-        <v>19</v>
+        <v>23.032258064516125</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -846,19 +893,19 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="4" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C18" s="5">
         <f>(C12*C13)/C7</f>
-        <v>57.736263736263737</v>
+        <v>1.8424793388429752</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="4" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F18" s="5">
         <f>(F12*F13)/C7</f>
-        <v>34.450549450549453</v>
+        <v>1.0623415977961432</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -866,19 +913,19 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="4" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5">
         <f>C18/2</f>
-        <v>28.868131868131869</v>
+        <v>0.92123966942148761</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="4" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="F19" s="5">
         <f>F18/2</f>
-        <v>17.225274725274726</v>
+        <v>0.53117079889807162</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -896,19 +943,19 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="4" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C21" s="5">
         <f>(C12*C14)/F7</f>
-        <v>114.21739130434783</v>
+        <v>9.582414151925077</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="4" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="F21" s="5">
         <f>(F12*F13)/F7</f>
-        <v>68.152173913043484</v>
+        <v>5.654398826979472</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -916,19 +963,19 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C22" s="7">
         <f>(C12*C14)/(2*F7)</f>
-        <v>57.108695652173914</v>
+        <v>4.7912070759625385</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F22" s="7">
         <f>(F12*F13)/(2*F7)</f>
-        <v>34.076086956521742</v>
+        <v>2.827199413489736</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -971,52 +1018,52 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C26" s="5">
         <f>(1/C13)*F1</f>
-        <v>6.6756756756756769E-2</v>
+        <v>5.0679405520169848E-2</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F26" s="5">
         <f>(1/F13)*F1</f>
-        <v>0.13</v>
+        <v>9.0991105463786526E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="4" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C27" s="5">
         <f>(C7/C13)*F1</f>
-        <v>0.60748648648648651</v>
+        <v>16.724203821656051</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F27" s="5">
         <f>(C7/F13)*F1</f>
-        <v>1.1830000000000001</v>
+        <v>30.027064803049555</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="4" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C28" s="5">
         <f>C27*2</f>
-        <v>1.214972972972973</v>
+        <v>33.448407643312102</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F28" s="5">
         <f>F27*2</f>
-        <v>2.3660000000000001</v>
+        <v>60.05412960609911</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1029,52 +1076,52 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="4" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C30" s="5">
         <f>(1/C14)*F1</f>
-        <v>6.6756756756756769E-2</v>
+        <v>5.1865844255975325E-2</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="F30" s="5">
         <f>(1/F14)*F1</f>
-        <v>0.13</v>
+        <v>9.4215686274509811E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C31" s="5">
         <f>(F7/C14)*F1</f>
-        <v>0.30708108108108106</v>
+        <v>3.2156823438704705</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="F31" s="5">
         <f>(F7/F14)*F1</f>
-        <v>0.59799999999999998</v>
+        <v>5.8413725490196091</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
       <c r="B32" s="6" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C32" s="7">
         <f>C31*2</f>
-        <v>0.61416216216216213</v>
+        <v>6.4313646877409409</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="F32" s="7">
         <f>F31*2</f>
-        <v>1.196</v>
+        <v>11.682745098039218</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1129,14 +1176,14 @@
       </c>
       <c r="C38" s="5">
         <f>(C36*C37)*C28</f>
-        <v>85.04810810810811</v>
+        <v>2341.3885350318469</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="5">
         <f>(F36*F37)*F28</f>
-        <v>165.62</v>
+        <v>4203.7890724269373</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1183,14 +1230,586 @@
       </c>
       <c r="C42" s="7">
         <f>(C40*C41)*C32</f>
-        <v>42.991351351351348</v>
+        <v>450.19552814186585</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F42" s="7">
         <f>(F40*F41)*F32</f>
-        <v>83.72</v>
+        <v>817.79215686274529</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="E35:F35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0D86B6-EC96-8645-917A-A9762B7FAD15}">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="E4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>9.1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <f>SUM(C5:C6)</f>
+        <v>9.1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7">
+        <f>SUM(F5:F6)</f>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="E9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5">
+        <v>43</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>37</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5">
+        <v>14.2</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5">
+        <f>((C10*(C5/C7))+(C11*(C6/C7)))</f>
+        <v>37</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5">
+        <f>((F10*(C5/C7))+(F11*(C6/C7)))</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8">
+        <f>((C10*(F5/F7))+(C11*(F6/F7)))</f>
+        <v>42.944272445820438</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="7">
+        <f>((F10*(F5/F7))+(F11*(F6/F7)))</f>
+        <v>23.953560371517028</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>(B9)</f>
+        <v>Ford Escape 2020 Hybrid</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="13" t="str">
+        <f>E9</f>
+        <v>Ford Escape 2008 XLT</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5">
+        <f>(C12*C13)/C7</f>
+        <v>57.736263736263737</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5">
+        <f>(F12*F13)/C7</f>
+        <v>34.450549450549453</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5">
+        <f>C18/2</f>
+        <v>28.868131868131869</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="5">
+        <f>F18/2</f>
+        <v>17.225274725274726</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="5">
+        <f>(C12*C14)/F7</f>
+        <v>1.8879525347698149</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="5">
+        <f>(F12*F13)/F7</f>
+        <v>0.97058823529411764</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="7">
+        <f>(C12*C14)/(2*F7)</f>
+        <v>0.94397626738490747</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="7">
+        <f>(F12*F13)/(2*F7)</f>
+        <v>0.48529411764705882</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>(B17)</f>
+        <v>Ford Escape 2020 Hybrid</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="E25" s="13" t="str">
+        <f>E17</f>
+        <v>Ford Escape 2008 XLT</v>
+      </c>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="5">
+        <f>(1/C13)*F1</f>
+        <v>6.2972972972972982E-2</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="5">
+        <f>(1/F13)*F1</f>
+        <v>0.12263157894736842</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5">
+        <f>(C7/C13)*F1</f>
+        <v>0.57305405405405407</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="5">
+        <f>(C7/F13)*F1</f>
+        <v>1.1159473684210526</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="5">
+        <f>C27*2</f>
+        <v>1.1461081081081081</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="5">
+        <f>F27*2</f>
+        <v>2.2318947368421052</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="5">
+        <f>(1/C14)*F1</f>
+        <v>5.4256362194506517E-2</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="5">
+        <f>(1/F14)*F1</f>
+        <v>9.7271552281245954E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="5">
+        <f>(F7/C14)*F1</f>
+        <v>17.524804988825604</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="5">
+        <f>(F7/F14)*F1</f>
+        <v>31.418711386842446</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="7">
+        <f>C31*2</f>
+        <v>35.049609977651208</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="7">
+        <f>F31*2</f>
+        <v>62.837422773684892</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <f>(B25)</f>
+        <v>Ford Escape 2020 Hybrid</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="E35" s="13" t="str">
+        <f>E25</f>
+        <v>Ford Escape 2008 XLT</v>
+      </c>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="5">
+        <v>70</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="5">
+        <f>(C36*C37)*C28</f>
+        <v>80.227567567567576</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="5">
+        <f>(F36*F37)*F28</f>
+        <v>156.23263157894735</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="5">
+        <v>70</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="5">
+        <v>1</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="7">
+        <f>(C40*C41)*C32</f>
+        <v>2453.4726984355848</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="7">
+        <f>(F40*F41)*F32</f>
+        <v>4398.6195941579426</v>
       </c>
     </row>
   </sheetData>
@@ -1212,12 +1831,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75FCCDA-06F2-ED44-BCD5-14D9E0756A90}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C462358-9A63-4D48-8958-D591B0DFAB04}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView zoomScale="169" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1237,7 +1856,7 @@
         <v>35</v>
       </c>
       <c r="F1" s="1">
-        <v>2.91</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1264,13 +1883,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>7.2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="5">
-        <v>6.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1279,13 +1898,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>4.3</v>
+        <v>9.1</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="5">
-        <v>2</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1295,14 +1914,14 @@
       </c>
       <c r="C7" s="7">
         <f>SUM(C5:C6)</f>
-        <v>11.5</v>
+        <v>9.1</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="7">
         <f>SUM(F5:F6)</f>
-        <v>8.8000000000000007</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1310,7 +1929,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="14"/>
       <c r="E9" s="13" t="s">
@@ -1324,7 +1943,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="5">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>7</v>
@@ -1339,7 +1958,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="5">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>8</v>
@@ -1354,7 +1973,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="5">
-        <v>15.1</v>
+        <v>14.2</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>9</v>
@@ -1370,14 +1989,14 @@
       </c>
       <c r="C13" s="5">
         <f>((C10*(C5/C7))+(C11*(C6/C7)))</f>
-        <v>26.382608695652173</v>
+        <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5">
         <f>((F10*(C5/C7))+(F11*(C6/C7)))</f>
-        <v>22.130434782608699</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1387,14 +2006,14 @@
       </c>
       <c r="C14" s="8">
         <f>((C10*(F5/F7))+(C11*(F6/F7)))</f>
-        <v>27.409090909090907</v>
+        <v>37</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="7">
         <f>((F10*(F5/F7))+(F11*(F6/F7)))</f>
-        <v>22.86363636363636</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1403,7 +2022,7 @@
       </c>
       <c r="B17" s="2" t="str">
         <f>(B9)</f>
-        <v>Ford Excape 2016 SE</v>
+        <v>Ford Escape 2020 Hybrid</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="9"/>
@@ -1422,7 +2041,7 @@
       </c>
       <c r="C18" s="5">
         <f>(C12*C13)/C7</f>
-        <v>34.641512287334592</v>
+        <v>57.736263736263737</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="4" t="s">
@@ -1430,7 +2049,7 @@
       </c>
       <c r="F18" s="5">
         <f>(F12*F13)/C7</f>
-        <v>31.752362948960307</v>
+        <v>34.450549450549453</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -1442,7 +2061,7 @@
       </c>
       <c r="C19" s="5">
         <f>C18/2</f>
-        <v>17.320756143667296</v>
+        <v>28.868131868131869</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="4" t="s">
@@ -1450,7 +2069,7 @@
       </c>
       <c r="F19" s="5">
         <f>F18/2</f>
-        <v>15.876181474480154</v>
+        <v>17.225274725274726</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -1472,7 +2091,7 @@
       </c>
       <c r="C21" s="5">
         <f>(C12*C14)/F7</f>
-        <v>47.031508264462801</v>
+        <v>114.21739130434783</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="4" t="s">
@@ -1480,7 +2099,7 @@
       </c>
       <c r="F21" s="5">
         <f>(F12*F13)/F7</f>
-        <v>41.494565217391312</v>
+        <v>68.152173913043484</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -1492,7 +2111,7 @@
       </c>
       <c r="C22" s="7">
         <f>(C12*C14)/(2*F7)</f>
-        <v>23.5157541322314</v>
+        <v>57.108695652173914</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="6" t="s">
@@ -1500,7 +2119,7 @@
       </c>
       <c r="F22" s="7">
         <f>(F12*F13)/(2*F7)</f>
-        <v>20.747282608695656</v>
+        <v>34.076086956521742</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -1531,7 +2150,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f>(B17)</f>
-        <v>Ford Excape 2016 SE</v>
+        <v>Ford Escape 2020 Hybrid</v>
       </c>
       <c r="C25" s="3"/>
       <c r="E25" s="13" t="str">
@@ -1547,14 +2166,14 @@
       </c>
       <c r="C26" s="5">
         <f>(1/C13)*F1</f>
-        <v>0.11029993408042189</v>
+        <v>5.7297297297297302E-2</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F26" s="5">
         <f>(1/F13)*F1</f>
-        <v>0.13149312377210215</v>
+        <v>0.11157894736842106</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1564,14 +2183,14 @@
       </c>
       <c r="C27" s="5">
         <f>(C7/C13)*F1</f>
-        <v>1.2684492419248516</v>
+        <v>0.52140540540540536</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="5">
         <f>(C7/F13)*F1</f>
-        <v>1.5121709233791745</v>
+        <v>1.0153684210526317</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1581,14 +2200,14 @@
       </c>
       <c r="C28" s="5">
         <f>C27*2</f>
-        <v>2.5368984838497033</v>
+        <v>1.0428108108108107</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="5">
         <f>F27*2</f>
-        <v>3.0243418467583489</v>
+        <v>2.0307368421052634</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1605,14 +2224,14 @@
       </c>
       <c r="C30" s="5">
         <f>(1/C14)*F1</f>
-        <v>0.10616915422885573</v>
+        <v>5.7297297297297302E-2</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="5">
         <f>(1/F14)*F1</f>
-        <v>0.12727634194831017</v>
+        <v>0.11157894736842106</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1622,14 +2241,14 @@
       </c>
       <c r="C31" s="5">
         <f>(F7/C14)*F1</f>
-        <v>0.93428855721393056</v>
+        <v>0.26356756756756755</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="5">
         <f>(F7/F14)*F1</f>
-        <v>1.1200318091451296</v>
+        <v>0.51326315789473687</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1639,14 +2258,14 @@
       </c>
       <c r="C32" s="7">
         <f>C31*2</f>
-        <v>1.8685771144278611</v>
+        <v>0.5271351351351351</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F32" s="7">
         <f>F31*2</f>
-        <v>2.2400636182902591</v>
+        <v>1.0265263157894737</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1655,7 +2274,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f>(B25)</f>
-        <v>Ford Excape 2016 SE</v>
+        <v>Ford Escape 2020 Hybrid</v>
       </c>
       <c r="C35" s="3"/>
       <c r="E35" s="13" t="str">
@@ -1685,13 +2304,13 @@
         <v>22</v>
       </c>
       <c r="C37" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F37" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1701,14 +2320,14 @@
       </c>
       <c r="C38" s="5">
         <f>(C36*C37)*C28</f>
-        <v>355.16578773895844</v>
+        <v>72.996756756756753</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="5">
         <f>(F36*F37)*F28</f>
-        <v>423.40785854616882</v>
+        <v>142.15157894736845</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1755,14 +2374,14 @@
       </c>
       <c r="C42" s="7">
         <f>(C40*C41)*C32</f>
-        <v>130.80039800995027</v>
+        <v>36.899459459459457</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F42" s="7">
         <f>(F40*F41)*F32</f>
-        <v>156.80445328031814</v>
+        <v>71.856842105263155</v>
       </c>
     </row>
   </sheetData>
@@ -1784,12 +2403,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD125E4E-57BC-7A4B-AC98-2F988CDDFCFF}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75FCCDA-06F2-ED44-BCD5-14D9E0756A90}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:F42"/>
+    <sheetView zoomScale="169" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1836,13 +2455,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>7.2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="5">
-        <v>6.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1851,13 +2470,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>4.3</v>
+        <v>9.1</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="5">
-        <v>2</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1867,14 +2486,14 @@
       </c>
       <c r="C7" s="7">
         <f>SUM(C5:C6)</f>
-        <v>11.5</v>
+        <v>9.1</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="7">
         <f>SUM(F5:F6)</f>
-        <v>8.8000000000000007</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1882,7 +2501,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C9" s="14"/>
       <c r="E9" s="13" t="s">
@@ -1911,7 +2530,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>8</v>
@@ -1926,7 +2545,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="5">
-        <v>15.3</v>
+        <v>15.1</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>9</v>
@@ -1942,14 +2561,14 @@
       </c>
       <c r="C13" s="5">
         <f>((C10*(C5/C7))+(C11*(C6/C7)))</f>
-        <v>27.130434782608695</v>
+        <v>22</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5">
         <f>((F10*(C5/C7))+(F11*(C6/C7)))</f>
-        <v>22.130434782608699</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1959,14 +2578,14 @@
       </c>
       <c r="C14" s="8">
         <f>((C10*(F5/F7))+(C11*(F6/F7)))</f>
-        <v>27.86363636363636</v>
+        <v>22</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="7">
         <f>((F10*(F5/F7))+(F11*(F6/F7)))</f>
-        <v>22.86363636363636</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1975,7 +2594,7 @@
       </c>
       <c r="B17" s="2" t="str">
         <f>(B9)</f>
-        <v>Mazda CX 5 2016 GT</v>
+        <v>Ford Excape 2016 SE</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="9"/>
@@ -1994,7 +2613,7 @@
       </c>
       <c r="C18" s="5">
         <f>(C12*C13)/C7</f>
-        <v>36.095274102079394</v>
+        <v>36.505494505494504</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="4" t="s">
@@ -2002,7 +2621,7 @@
       </c>
       <c r="F18" s="5">
         <f>(F12*F13)/C7</f>
-        <v>31.752362948960307</v>
+        <v>34.450549450549453</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -2014,7 +2633,7 @@
       </c>
       <c r="C19" s="5">
         <f>C18/2</f>
-        <v>18.047637051039697</v>
+        <v>18.252747252747252</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="4" t="s">
@@ -2022,7 +2641,7 @@
       </c>
       <c r="F19" s="5">
         <f>F18/2</f>
-        <v>15.876181474480154</v>
+        <v>17.225274725274726</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -2044,7 +2663,7 @@
       </c>
       <c r="C21" s="5">
         <f>(C12*C14)/F7</f>
-        <v>48.444731404958667</v>
+        <v>72.217391304347828</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="4" t="s">
@@ -2052,7 +2671,7 @@
       </c>
       <c r="F21" s="5">
         <f>(F12*F13)/F7</f>
-        <v>41.494565217391312</v>
+        <v>68.152173913043484</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -2064,7 +2683,7 @@
       </c>
       <c r="C22" s="7">
         <f>(C12*C14)/(2*F7)</f>
-        <v>24.222365702479333</v>
+        <v>36.108695652173914</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="6" t="s">
@@ -2072,7 +2691,7 @@
       </c>
       <c r="F22" s="7">
         <f>(F12*F13)/(2*F7)</f>
-        <v>20.747282608695656</v>
+        <v>34.076086956521742</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -2103,7 +2722,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f>(B17)</f>
-        <v>Mazda CX 5 2016 GT</v>
+        <v>Ford Excape 2016 SE</v>
       </c>
       <c r="C25" s="3"/>
       <c r="E25" s="13" t="str">
@@ -2119,14 +2738,14 @@
       </c>
       <c r="C26" s="5">
         <f>(1/C13)*F1</f>
-        <v>0.1072596153846154</v>
+        <v>0.13227272727272729</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F26" s="5">
         <f>(1/F13)*F1</f>
-        <v>0.13149312377210215</v>
+        <v>0.1531578947368421</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -2136,14 +2755,14 @@
       </c>
       <c r="C27" s="5">
         <f>(C7/C13)*F1</f>
-        <v>1.233485576923077</v>
+        <v>1.2036818181818183</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="5">
         <f>(C7/F13)*F1</f>
-        <v>1.5121709233791745</v>
+        <v>1.3937368421052632</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -2153,14 +2772,14 @@
       </c>
       <c r="C28" s="5">
         <f>C27*2</f>
-        <v>2.4669711538461541</v>
+        <v>2.4073636363636366</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="5">
         <f>F27*2</f>
-        <v>3.0243418467583489</v>
+        <v>2.7874736842105263</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -2177,14 +2796,14 @@
       </c>
       <c r="C30" s="5">
         <f>(1/C14)*F1</f>
-        <v>0.10443719412724309</v>
+        <v>0.13227272727272729</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="5">
         <f>(1/F14)*F1</f>
-        <v>0.12727634194831017</v>
+        <v>0.1531578947368421</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -2194,14 +2813,14 @@
       </c>
       <c r="C31" s="5">
         <f>(F7/C14)*F1</f>
-        <v>0.91904730831973924</v>
+        <v>0.60845454545454547</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="5">
         <f>(F7/F14)*F1</f>
-        <v>1.1200318091451296</v>
+        <v>0.70452631578947367</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -2211,14 +2830,14 @@
       </c>
       <c r="C32" s="7">
         <f>C31*2</f>
-        <v>1.8380946166394785</v>
+        <v>1.2169090909090909</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F32" s="7">
         <f>F31*2</f>
-        <v>2.2400636182902591</v>
+        <v>1.4090526315789473</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2227,7 +2846,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f>(B25)</f>
-        <v>Mazda CX 5 2016 GT</v>
+        <v>Ford Excape 2016 SE</v>
       </c>
       <c r="C35" s="3"/>
       <c r="E35" s="13" t="str">
@@ -2273,14 +2892,14 @@
       </c>
       <c r="C38" s="5">
         <f>(C36*C37)*C28</f>
-        <v>345.37596153846158</v>
+        <v>337.03090909090912</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="5">
         <f>(F36*F37)*F28</f>
-        <v>423.40785854616882</v>
+        <v>390.24631578947367</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2327,14 +2946,14 @@
       </c>
       <c r="C42" s="7">
         <f>(C40*C41)*C32</f>
-        <v>128.66662316476351</v>
+        <v>85.183636363636367</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F42" s="7">
         <f>(F40*F41)*F32</f>
-        <v>156.80445328031814</v>
+        <v>98.633684210526312</v>
       </c>
     </row>
   </sheetData>
@@ -2356,12 +2975,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4C0E1F-D170-C44C-88B9-EC92D9166A09}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD125E4E-57BC-7A4B-AC98-2F988CDDFCFF}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2408,13 +3027,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>7.2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="5">
-        <v>6.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2423,13 +3042,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>4.3</v>
+        <v>9.1</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="5">
-        <v>2</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2439,14 +3058,14 @@
       </c>
       <c r="C7" s="7">
         <f>SUM(C5:C6)</f>
-        <v>11.5</v>
+        <v>9.1</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="7">
         <f>SUM(F5:F6)</f>
-        <v>8.8000000000000007</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2454,7 +3073,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C9" s="14"/>
       <c r="E9" s="13" t="s">
@@ -2468,7 +3087,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="5">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>7</v>
@@ -2483,7 +3102,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="5">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>8</v>
@@ -2498,7 +3117,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="5">
-        <v>11.9</v>
+        <v>15.3</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>9</v>
@@ -2514,14 +3133,14 @@
       </c>
       <c r="C13" s="5">
         <f>((C10*(C5/C7))+(C11*(C6/C7)))</f>
-        <v>30.130434782608695</v>
+        <v>24</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5">
         <f>((F10*(C5/C7))+(F11*(C6/C7)))</f>
-        <v>22.130434782608699</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2531,14 +3150,14 @@
       </c>
       <c r="C14" s="8">
         <f>((C10*(F5/F7))+(C11*(F6/F7)))</f>
-        <v>30.86363636363636</v>
+        <v>24</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="7">
         <f>((F10*(F5/F7))+(F11*(F6/F7)))</f>
-        <v>22.86363636363636</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -2547,7 +3166,7 @@
       </c>
       <c r="B17" s="2" t="str">
         <f>(B9)</f>
-        <v>Mazda CX 3 2016 GT</v>
+        <v>Mazda CX 5 2016 GT</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="9"/>
@@ -2566,7 +3185,7 @@
       </c>
       <c r="C18" s="5">
         <f>(C12*C13)/C7</f>
-        <v>31.17844990548204</v>
+        <v>40.351648351648358</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="4" t="s">
@@ -2574,7 +3193,7 @@
       </c>
       <c r="F18" s="5">
         <f>(F12*F13)/C7</f>
-        <v>31.752362948960307</v>
+        <v>34.450549450549453</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -2586,7 +3205,7 @@
       </c>
       <c r="C19" s="5">
         <f>C18/2</f>
-        <v>15.58922495274102</v>
+        <v>20.175824175824179</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="4" t="s">
@@ -2594,7 +3213,7 @@
       </c>
       <c r="F19" s="5">
         <f>F18/2</f>
-        <v>15.876181474480154</v>
+        <v>17.225274725274726</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -2616,7 +3235,7 @@
       </c>
       <c r="C21" s="5">
         <f>(C12*C14)/F7</f>
-        <v>41.736053719008261</v>
+        <v>79.826086956521749</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="4" t="s">
@@ -2624,7 +3243,7 @@
       </c>
       <c r="F21" s="5">
         <f>(F12*F13)/F7</f>
-        <v>41.494565217391312</v>
+        <v>68.152173913043484</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -2636,7 +3255,7 @@
       </c>
       <c r="C22" s="7">
         <f>(C12*C14)/(2*F7)</f>
-        <v>20.86802685950413</v>
+        <v>39.913043478260875</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="6" t="s">
@@ -2644,7 +3263,7 @@
       </c>
       <c r="F22" s="7">
         <f>(F12*F13)/(2*F7)</f>
-        <v>20.747282608695656</v>
+        <v>34.076086956521742</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -2675,7 +3294,7 @@
       </c>
       <c r="B25" s="2" t="str">
         <f>(B17)</f>
-        <v>Mazda CX 3 2016 GT</v>
+        <v>Mazda CX 5 2016 GT</v>
       </c>
       <c r="C25" s="3"/>
       <c r="E25" s="13" t="str">
@@ -2691,14 +3310,14 @@
       </c>
       <c r="C26" s="5">
         <f>(1/C13)*F1</f>
-        <v>9.6580086580086585E-2</v>
+        <v>0.12125</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F26" s="5">
         <f>(1/F13)*F1</f>
-        <v>0.13149312377210215</v>
+        <v>0.1531578947368421</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -2708,14 +3327,14 @@
       </c>
       <c r="C27" s="5">
         <f>(C7/C13)*F1</f>
-        <v>1.1106709956709957</v>
+        <v>1.103375</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="5">
         <f>(C7/F13)*F1</f>
-        <v>1.5121709233791745</v>
+        <v>1.3937368421052632</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -2725,14 +3344,14 @@
       </c>
       <c r="C28" s="5">
         <f>C27*2</f>
-        <v>2.2213419913419914</v>
+        <v>2.20675</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="5">
         <f>F27*2</f>
-        <v>3.0243418467583489</v>
+        <v>2.7874736842105263</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -2749,14 +3368,14 @@
       </c>
       <c r="C30" s="5">
         <f>(1/C14)*F1</f>
-        <v>9.4285714285714292E-2</v>
+        <v>0.12125</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="5">
         <f>(1/F14)*F1</f>
-        <v>0.12727634194831017</v>
+        <v>0.1531578947368421</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -2766,14 +3385,14 @@
       </c>
       <c r="C31" s="5">
         <f>(F7/C14)*F1</f>
-        <v>0.82971428571428585</v>
+        <v>0.55774999999999997</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="5">
         <f>(F7/F14)*F1</f>
-        <v>1.1200318091451296</v>
+        <v>0.70452631578947367</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -2783,14 +3402,14 @@
       </c>
       <c r="C32" s="7">
         <f>C31*2</f>
-        <v>1.6594285714285717</v>
+        <v>1.1154999999999999</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F32" s="7">
         <f>F31*2</f>
-        <v>2.2400636182902591</v>
+        <v>1.4090526315789473</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2799,7 +3418,7 @@
       </c>
       <c r="B35" s="2" t="str">
         <f>(B25)</f>
-        <v>Mazda CX 3 2016 GT</v>
+        <v>Mazda CX 5 2016 GT</v>
       </c>
       <c r="C35" s="3"/>
       <c r="E35" s="13" t="str">
@@ -2845,14 +3464,14 @@
       </c>
       <c r="C38" s="5">
         <f>(C36*C37)*C28</f>
-        <v>310.9878787878788</v>
+        <v>308.94499999999999</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="5">
         <f>(F36*F37)*F28</f>
-        <v>423.40785854616882</v>
+        <v>390.24631578947367</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2899,30 +3518,602 @@
       </c>
       <c r="C42" s="7">
         <f>(C40*C41)*C32</f>
-        <v>116.16000000000003</v>
+        <v>78.084999999999994</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F42" s="7">
         <f>(F40*F41)*F32</f>
-        <v>156.80445328031814</v>
+        <v>98.633684210526312</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="A25:A32"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="E35:F35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4C0E1F-D170-C44C-88B9-EC92D9166A09}">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>9.1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <f>SUM(C5:C6)</f>
+        <v>9.1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7">
+        <f>SUM(F5:F6)</f>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="E9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>27</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5">
+        <v>11.9</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5">
+        <f>((C10*(C5/C7))+(C11*(C6/C7)))</f>
+        <v>27</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5">
+        <f>((F10*(C5/C7))+(F11*(C6/C7)))</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8">
+        <f>((C10*(F5/F7))+(C11*(F6/F7)))</f>
+        <v>27</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="7">
+        <f>((F10*(F5/F7))+(F11*(F6/F7)))</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>(B9)</f>
+        <v>Mazda CX 3 2016 GT</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="13" t="str">
+        <f>E9</f>
+        <v>Ford Escape 2008 XLT</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5">
+        <f>(C12*C13)/C7</f>
+        <v>35.307692307692314</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5">
+        <f>(F12*F13)/C7</f>
+        <v>34.450549450549453</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5">
+        <f>C18/2</f>
+        <v>17.653846153846157</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="5">
+        <f>F18/2</f>
+        <v>17.225274725274726</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="5">
+        <f>(C12*C14)/F7</f>
+        <v>69.84782608695653</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="5">
+        <f>(F12*F13)/F7</f>
+        <v>68.152173913043484</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="7">
+        <f>(C12*C14)/(2*F7)</f>
+        <v>34.923913043478265</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="7">
+        <f>(F12*F13)/(2*F7)</f>
+        <v>34.076086956521742</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>(B17)</f>
+        <v>Mazda CX 3 2016 GT</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="E25" s="13" t="str">
+        <f>E17</f>
+        <v>Ford Escape 2008 XLT</v>
+      </c>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="5">
+        <f>(1/C13)*F1</f>
+        <v>7.8518518518518515E-2</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="5">
+        <f>(1/F13)*F1</f>
+        <v>0.11157894736842106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5">
+        <f>(C7/C13)*F1</f>
+        <v>0.71451851851851855</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="5">
+        <f>(C7/F13)*F1</f>
+        <v>1.0153684210526317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="5">
+        <f>C27*2</f>
+        <v>1.4290370370370371</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="5">
+        <f>F27*2</f>
+        <v>2.0307368421052634</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="5">
+        <f>(1/C14)*F1</f>
+        <v>7.8518518518518515E-2</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="5">
+        <f>(1/F14)*F1</f>
+        <v>0.11157894736842106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="5">
+        <f>(F7/C14)*F1</f>
+        <v>0.36118518518518522</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="5">
+        <f>(F7/F14)*F1</f>
+        <v>0.51326315789473687</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="7">
+        <f>C31*2</f>
+        <v>0.72237037037037044</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="7">
+        <f>F31*2</f>
+        <v>1.0265263157894737</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <f>(B25)</f>
+        <v>Mazda CX 3 2016 GT</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="E35" s="13" t="str">
+        <f>E25</f>
+        <v>Ford Escape 2008 XLT</v>
+      </c>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="5">
+        <v>70</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="5">
+        <f>(C36*C37)*C28</f>
+        <v>200.06518518518519</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="5">
+        <f>(F36*F37)*F28</f>
+        <v>284.3031578947369</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="5">
+        <v>70</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="5">
+        <v>1</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="7">
+        <f>(C40*C41)*C32</f>
+        <v>50.565925925925931</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="7">
+        <f>(F40*F41)*F32</f>
+        <v>71.856842105263155</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="E35:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>